<commit_message>
add code for cham cong function
</commit_message>
<xml_diff>
--- a/notion_data/LUY_KE_NGAY_HE_THONG.xlsx
+++ b/notion_data/LUY_KE_NGAY_HE_THONG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY137"/>
+  <dimension ref="A1:AY138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,17 +698,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>f731208e-1075-48d0-abc5-8db88eae20bb</t>
+          <t>0ac9b051-5cc9-406d-93cd-dfd30b94f1b9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-04T03:59:00.000Z</t>
+          <t>2024-07-06T08:53:00.000Z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -721,7 +721,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://www.notion.so/1-f731208e107548d0abc58db88eae20bb</t>
+          <t>https://www.notion.so/1-0ac9b0515cc9406d93cddfd30b94f1b9</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -915,17 +915,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>25114a41-1915-4ca5-b664-936891b3097b</t>
+          <t>f731208e-1075-48d0-abc5-8db88eae20bb</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-07-02T21:33:00.000Z</t>
+          <t>2024-07-04T03:59:00.000Z</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://www.notion.so/2-25114a4119154ca5b664936891b3097b</t>
+          <t>https://www.notion.so/2-f731208e107548d0abc58db88eae20bb</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -1132,17 +1132,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>fab28d7f-b767-4c78-bded-853d1a301515</t>
+          <t>25114a41-1915-4ca5-b664-936891b3097b</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-07-02T03:00:00.000Z</t>
+          <t>2024-07-02T21:33:00.000Z</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.notion.so/3-fab28d7fb7674c78bded853d1a301515</t>
+          <t>https://www.notion.so/3-25114a4119154ca5b664936891b3097b</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -1349,17 +1349,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>706d4f2c-a2ec-4c18-a2c5-5935e3f1599c</t>
+          <t>fab28d7f-b767-4c78-bded-853d1a301515</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-07-01T04:20:00.000Z</t>
+          <t>2024-07-02T03:00:00.000Z</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.notion.so/4-706d4f2ca2ec4c18a2c55935e3f1599c</t>
+          <t>https://www.notion.so/4-fab28d7fb7674c78bded853d1a301515</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>daa8de3a-ff76-447f-8245-aba8917006f2</t>
+          <t>706d4f2c-a2ec-4c18-a2c5-5935e3f1599c</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-06-30T09:10:00.000Z</t>
+          <t>2024-07-01T04:20:00.000Z</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.notion.so/5-daa8de3aff76447f8245aba8917006f2</t>
+          <t>https://www.notion.so/5-706d4f2ca2ec4c18a2c55935e3f1599c</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1783,17 +1783,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>d77a665d-eebe-444c-b4cf-26b67b4604df</t>
+          <t>daa8de3a-ff76-447f-8245-aba8917006f2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-06-29T09:35:00.000Z</t>
+          <t>2024-06-30T09:10:00.000Z</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.notion.so/6-d77a665deebe444cb4cf26b67b4604df</t>
+          <t>https://www.notion.so/6-daa8de3aff76447f8245aba8917006f2</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -2000,17 +2000,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>551b8192-7e28-4d6d-b116-e2e40a5283c3</t>
+          <t>d77a665d-eebe-444c-b4cf-26b67b4604df</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-06-28T14:00:00.000Z</t>
+          <t>2024-06-29T09:35:00.000Z</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.notion.so/7-551b81927e284d6db116e2e40a5283c3</t>
+          <t>https://www.notion.so/7-d77a665deebe444cb4cf26b67b4604df</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -2217,17 +2217,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5b3dd329-4293-42b5-80e0-1330f7e5d77b</t>
+          <t>551b8192-7e28-4d6d-b116-e2e40a5283c3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-06-27T05:19:00.000Z</t>
+          <t>2024-06-28T14:00:00.000Z</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.notion.so/8-5b3dd329429342b580e01330f7e5d77b</t>
+          <t>https://www.notion.so/8-551b81927e284d6db116e2e40a5283c3</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -2434,17 +2434,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>420881fe-5a64-41f5-83c7-4c39413c8d8d</t>
+          <t>5b3dd329-4293-42b5-80e0-1330f7e5d77b</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-06-26T11:55:00.000Z</t>
+          <t>2024-06-27T05:19:00.000Z</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.notion.so/9-420881fe5a6441f583c74c39413c8d8d</t>
+          <t>https://www.notion.so/9-5b3dd329429342b580e01330f7e5d77b</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -2651,17 +2651,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>61c88664-13a8-48a3-b0c6-0c943ec81d24</t>
+          <t>420881fe-5a64-41f5-83c7-4c39413c8d8d</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2024-06-25T15:21:00.000Z</t>
+          <t>2024-06-26T11:55:00.000Z</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.notion.so/10-61c8866413a848a3b0c60c943ec81d24</t>
+          <t>https://www.notion.so/10-420881fe5a6441f583c74c39413c8d8d</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3ffcb89f-55d1-477e-a58a-a80a3a054b47</t>
+          <t>61c88664-13a8-48a3-b0c6-0c943ec81d24</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.notion.so/11-3ffcb89f55d1477ea58aa80a3a054b47</t>
+          <t>https://www.notion.so/11-61c8866413a848a3b0c60c943ec81d24</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -3085,17 +3085,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>646614a9-9864-4cdc-a72b-2283914acefd</t>
+          <t>3ffcb89f-55d1-477e-a58a-a80a3a054b47</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2024-06-25T15:18:00.000Z</t>
+          <t>2024-06-25T15:21:00.000Z</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.notion.so/12-646614a998644cdca72b2283914acefd</t>
+          <t>https://www.notion.so/12-3ffcb89f55d1477ea58aa80a3a054b47</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -3302,17 +3302,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>e25ff82f-b3c8-4162-94da-26962c577e6f</t>
+          <t>646614a9-9864-4cdc-a72b-2283914acefd</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2024-06-25T09:40:00.000Z</t>
+          <t>2024-06-25T15:18:00.000Z</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.notion.so/13-e25ff82fb3c8416294da26962c577e6f</t>
+          <t>https://www.notion.so/13-646614a998644cdca72b2283914acefd</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -3519,17 +3519,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2e4df6af-ce7f-438e-9d21-8b42888787d8</t>
+          <t>e25ff82f-b3c8-4162-94da-26962c577e6f</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024-06-25T09:39:00.000Z</t>
+          <t>2024-06-25T09:40:00.000Z</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://www.notion.so/14-2e4df6afce7f438e9d218b42888787d8</t>
+          <t>https://www.notion.so/14-e25ff82fb3c8416294da26962c577e6f</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -3736,17 +3736,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b344bc3e-71f3-43e5-a7c8-a845ae0c8270</t>
+          <t>2e4df6af-ce7f-438e-9d21-8b42888787d8</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024-06-25T03:13:00.000Z</t>
+          <t>2024-06-25T09:39:00.000Z</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://www.notion.so/15-b344bc3e71f343e5a7c8a845ae0c8270</t>
+          <t>https://www.notion.so/15-2e4df6afce7f438e9d218b42888787d8</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>796b1251-3d1b-4215-8601-eaff4e7c9b68</t>
+          <t>b344bc3e-71f3-43e5-a7c8-a845ae0c8270</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://www.notion.so/16-796b12513d1b42158601eaff4e7c9b68</t>
+          <t>https://www.notion.so/16-b344bc3e71f343e5a7c8a845ae0c8270</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -4170,7 +4170,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2dbf23bc-96b5-4c45-a032-449de4fc6c2a</t>
+          <t>796b1251-3d1b-4215-8601-eaff4e7c9b68</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://www.notion.so/17-2dbf23bc96b54c45a032449de4fc6c2a</t>
+          <t>https://www.notion.so/17-796b12513d1b42158601eaff4e7c9b68</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>fb9c5676-a808-4dc6-bd44-e309dbce5fa5</t>
+          <t>2dbf23bc-96b5-4c45-a032-449de4fc6c2a</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://www.notion.so/18-fb9c5676a8084dc6bd44e309dbce5fa5</t>
+          <t>https://www.notion.so/18-2dbf23bc96b54c45a032449de4fc6c2a</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -4604,17 +4604,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7add5d63-cce1-4eac-b365-f50e7e00b6cc</t>
+          <t>fb9c5676-a808-4dc6-bd44-e309dbce5fa5</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2024-06-25T03:05:00.000Z</t>
+          <t>2024-06-25T03:13:00.000Z</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4627,7 +4627,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://www.notion.so/19-7add5d63cce14eacb365f50e7e00b6cc</t>
+          <t>https://www.notion.so/19-fb9c5676a8084dc6bd44e309dbce5fa5</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>df53934a-e5df-452d-9863-bf6f9fab085a</t>
+          <t>7add5d63-cce1-4eac-b365-f50e7e00b6cc</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4831,7 +4831,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://www.notion.so/20-df53934ae5df452d9863bf6f9fab085a</t>
+          <t>https://www.notion.so/20-7add5d63cce14eacb365f50e7e00b6cc</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0aed403a-3958-4747-8783-e2f73cd45ddf</t>
+          <t>df53934a-e5df-452d-9863-bf6f9fab085a</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -5048,7 +5048,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -5061,7 +5061,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://www.notion.so/21-0aed403a395847478783e2f73cd45ddf</t>
+          <t>https://www.notion.so/21-df53934ae5df452d9863bf6f9fab085a</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -5255,7 +5255,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>a16a55af-6817-4200-bc41-0f5dcc98fe8b</t>
+          <t>0aed403a-3958-4747-8783-e2f73cd45ddf</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://www.notion.so/22-a16a55af68174200bc410f5dcc98fe8b</t>
+          <t>https://www.notion.so/22-0aed403a395847478783e2f73cd45ddf</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
@@ -5472,7 +5472,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>bf91e048-d329-45d1-a14b-095345a737bf</t>
+          <t>a16a55af-6817-4200-bc41-0f5dcc98fe8b</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -5482,7 +5482,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://www.notion.so/23-bf91e048d32945d1a14b095345a737bf</t>
+          <t>https://www.notion.so/23-a16a55af68174200bc410f5dcc98fe8b</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
@@ -5689,17 +5689,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ceda31bf-563b-49de-b855-66a69556885b</t>
+          <t>bf91e048-d329-45d1-a14b-095345a737bf</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2024-06-25T02:57:00.000Z</t>
+          <t>2024-06-25T03:05:00.000Z</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -5712,7 +5712,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://www.notion.so/24-ceda31bf563b49deb85566a69556885b</t>
+          <t>https://www.notion.so/24-bf91e048d32945d1a14b095345a737bf</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -5906,17 +5906,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>e5fa84a6-7667-4817-a52c-04e5e9d9df48</t>
+          <t>ceda31bf-563b-49de-b855-66a69556885b</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2024-06-25T01:56:00.000Z</t>
+          <t>2024-06-25T02:57:00.000Z</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -5929,7 +5929,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://www.notion.so/25-e5fa84a676674817a52c04e5e9d9df48</t>
+          <t>https://www.notion.so/25-ceda31bf563b49deb85566a69556885b</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3cc93476-770c-4fc5-8fb7-bf19e4366bc4</t>
+          <t>e5fa84a6-7667-4817-a52c-04e5e9d9df48</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -6133,7 +6133,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://www.notion.so/26-3cc93476770c4fc58fb7bf19e4366bc4</t>
+          <t>https://www.notion.so/26-e5fa84a676674817a52c04e5e9d9df48</t>
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
@@ -6340,7 +6340,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0c1b1ed1-b38c-4740-a6b0-aa5e306bc997</t>
+          <t>3cc93476-770c-4fc5-8fb7-bf19e4366bc4</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -6350,7 +6350,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -6363,7 +6363,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://www.notion.so/27-0c1b1ed1b38c4740a6b0aa5e306bc997</t>
+          <t>https://www.notion.so/27-3cc93476770c4fc58fb7bf19e4366bc4</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>86ae44bf-42e6-4c7f-8b13-fa13cb822124</t>
+          <t>0c1b1ed1-b38c-4740-a6b0-aa5e306bc997</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://www.notion.so/28-86ae44bf42e64c7f8b13fa13cb822124</t>
+          <t>https://www.notion.so/28-0c1b1ed1b38c4740a6b0aa5e306bc997</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
@@ -6774,7 +6774,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>c97267f7-485c-4680-8a95-6bcb55a38d89</t>
+          <t>86ae44bf-42e6-4c7f-8b13-fa13cb822124</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -6784,7 +6784,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://www.notion.so/29-c97267f7485c46808a956bcb55a38d89</t>
+          <t>https://www.notion.so/29-86ae44bf42e64c7f8b13fa13cb822124</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
@@ -6991,7 +6991,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8153333a-011b-4919-820f-d1f2f6dbbf5e</t>
+          <t>c97267f7-485c-4680-8a95-6bcb55a38d89</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -7014,7 +7014,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://www.notion.so/30-8153333a011b4919820fd1f2f6dbbf5e</t>
+          <t>https://www.notion.so/30-c97267f7485c46808a956bcb55a38d89</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8de44170-ec9c-4bcc-8a82-2fc568a0a386</t>
+          <t>8153333a-011b-4919-820f-d1f2f6dbbf5e</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -7218,7 +7218,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -7231,7 +7231,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://www.notion.so/31-8de44170ec9c4bcc8a822fc568a0a386</t>
+          <t>https://www.notion.so/31-8153333a011b4919820fd1f2f6dbbf5e</t>
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>91e54e88-ea6e-4842-81dd-e151ce52dc9d</t>
+          <t>8de44170-ec9c-4bcc-8a82-2fc568a0a386</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -7435,7 +7435,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -7448,7 +7448,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://www.notion.so/32-91e54e88ea6e484281dde151ce52dc9d</t>
+          <t>https://www.notion.so/32-8de44170ec9c4bcc8a822fc568a0a386</t>
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
@@ -7642,7 +7642,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1915e040-0fa9-45a5-b113-a9c400d8a035</t>
+          <t>91e54e88-ea6e-4842-81dd-e151ce52dc9d</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -7652,7 +7652,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -7665,7 +7665,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>https://www.notion.so/33-1915e0400fa945a5b113a9c400d8a035</t>
+          <t>https://www.notion.so/33-91e54e88ea6e484281dde151ce52dc9d</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
@@ -7859,7 +7859,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>9601e83d-fa3c-4426-9d40-3c91776cd0a5</t>
+          <t>1915e040-0fa9-45a5-b113-a9c400d8a035</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -7869,7 +7869,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -7882,7 +7882,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>https://www.notion.so/34-9601e83dfa3c44269d403c91776cd0a5</t>
+          <t>https://www.notion.so/34-1915e0400fa945a5b113a9c400d8a035</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
@@ -8076,17 +8076,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>600a3c5b-b714-40ea-91a4-c53230e174a4</t>
+          <t>9601e83d-fa3c-4426-9d40-3c91776cd0a5</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2024-06-25T01:55:00.000Z</t>
+          <t>2024-06-25T01:56:00.000Z</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -8099,7 +8099,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>https://www.notion.so/35-600a3c5bb71440ea91a4c53230e174a4</t>
+          <t>https://www.notion.so/35-9601e83dfa3c44269d403c91776cd0a5</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>0819d336-e046-4aa9-a68c-74d8734f111b</t>
+          <t>600a3c5b-b714-40ea-91a4-c53230e174a4</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -8316,7 +8316,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>https://www.notion.so/36-0819d336e0464aa9a68c74d8734f111b</t>
+          <t>https://www.notion.so/36-600a3c5bb71440ea91a4c53230e174a4</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -8510,7 +8510,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>f6c48f5e-2ea1-4442-994d-00dd050d7573</t>
+          <t>0819d336-e046-4aa9-a68c-74d8734f111b</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -8520,7 +8520,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -8533,7 +8533,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://www.notion.so/37-f6c48f5e2ea14442994d00dd050d7573</t>
+          <t>https://www.notion.so/37-0819d336e0464aa9a68c74d8734f111b</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>fea89f72-9297-429c-872e-5f22167f0ddd</t>
+          <t>f6c48f5e-2ea1-4442-994d-00dd050d7573</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -8737,7 +8737,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:10:00.000Z</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -8750,7 +8750,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://www.notion.so/38-fea89f729297429c872e5f22167f0ddd</t>
+          <t>https://www.notion.so/38-f6c48f5e2ea14442994d00dd050d7573</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>415678f2-6740-428a-b0ff-ac64f3b76690</t>
+          <t>fea89f72-9297-429c-872e-5f22167f0ddd</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -8954,7 +8954,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -8967,7 +8967,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>https://www.notion.so/39-415678f26740428ab0ffac64f3b76690</t>
+          <t>https://www.notion.so/39-fea89f729297429c872e5f22167f0ddd</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -9161,7 +9161,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ef8d636c-57ef-4df9-b102-21ff62a18e37</t>
+          <t>415678f2-6740-428a-b0ff-ac64f3b76690</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -9171,7 +9171,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -9184,7 +9184,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>https://www.notion.so/40-ef8d636c57ef4df9b10221ff62a18e37</t>
+          <t>https://www.notion.so/40-415678f26740428ab0ffac64f3b76690</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
@@ -9378,17 +9378,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>9dd551e6-e5cf-4813-b4ab-304e4734155a</t>
+          <t>ef8d636c-57ef-4df9-b102-21ff62a18e37</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2024-06-25T01:43:00.000Z</t>
+          <t>2024-06-25T01:55:00.000Z</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -9401,7 +9401,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>https://www.notion.so/41-9dd551e6e5cf4813b4ab304e4734155a</t>
+          <t>https://www.notion.so/41-ef8d636c57ef4df9b10221ff62a18e37</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -9595,7 +9595,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>488babcc-5d0a-452d-a424-45df5507a6e3</t>
+          <t>9dd551e6-e5cf-4813-b4ab-304e4734155a</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -9605,7 +9605,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -9618,7 +9618,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>https://www.notion.so/42-488babcc5d0a452da42445df5507a6e3</t>
+          <t>https://www.notion.so/42-9dd551e6e5cf4813b4ab304e4734155a</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -9812,7 +9812,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>e9dbc2c7-a16d-43de-bad1-264d033dd2f3</t>
+          <t>488babcc-5d0a-452d-a424-45df5507a6e3</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -9822,7 +9822,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -9835,7 +9835,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>https://www.notion.so/43-e9dbc2c7a16d43debad1264d033dd2f3</t>
+          <t>https://www.notion.so/43-488babcc5d0a452da42445df5507a6e3</t>
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
@@ -10029,7 +10029,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>be62e55e-9269-4581-a2f7-4dd68fe99cbd</t>
+          <t>e9dbc2c7-a16d-43de-bad1-264d033dd2f3</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -10039,7 +10039,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -10052,7 +10052,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>https://www.notion.so/44-be62e55e92694581a2f74dd68fe99cbd</t>
+          <t>https://www.notion.so/44-e9dbc2c7a16d43debad1264d033dd2f3</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -10246,17 +10246,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>d9c1e1c3-0688-425c-8f9b-6606145353b9</t>
+          <t>be62e55e-9269-4581-a2f7-4dd68fe99cbd</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2024-06-24T17:12:00.000Z</t>
+          <t>2024-06-25T01:43:00.000Z</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -10269,7 +10269,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>https://www.notion.so/45-d9c1e1c30688425c8f9b6606145353b9</t>
+          <t>https://www.notion.so/45-be62e55e92694581a2f74dd68fe99cbd</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
@@ -10463,7 +10463,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1b7af46b-d075-4d07-8e3d-34b70d11ed6a</t>
+          <t>d9c1e1c3-0688-425c-8f9b-6606145353b9</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -10473,7 +10473,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -10486,7 +10486,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>https://www.notion.so/46-1b7af46bd0754d078e3d34b70d11ed6a</t>
+          <t>https://www.notion.so/46-d9c1e1c30688425c8f9b6606145353b9</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -10680,7 +10680,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>05ea37ab-6a1f-4b85-8cf7-3837087e14c6</t>
+          <t>1b7af46b-d075-4d07-8e3d-34b70d11ed6a</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -10690,7 +10690,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>https://www.notion.so/47-05ea37ab6a1f4b858cf73837087e14c6</t>
+          <t>https://www.notion.so/47-1b7af46bd0754d078e3d34b70d11ed6a</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
@@ -10897,7 +10897,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>f9b6d9fb-9f0b-4c27-850a-3096e797aada</t>
+          <t>05ea37ab-6a1f-4b85-8cf7-3837087e14c6</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -10907,7 +10907,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2024-07-04T09:47:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -10920,7 +10920,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>https://www.notion.so/48-f9b6d9fb9f0b4c27850a3096e797aada</t>
+          <t>https://www.notion.so/48-05ea37ab6a1f4b858cf73837087e14c6</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -11114,7 +11114,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>b91a1bc1-abbc-41ae-8f1c-5115ed8c076b</t>
+          <t>f9b6d9fb-9f0b-4c27-850a-3096e797aada</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -11124,7 +11124,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -11137,7 +11137,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>https://www.notion.so/49-b91a1bc1abbc41ae8f1c5115ed8c076b</t>
+          <t>https://www.notion.so/49-f9b6d9fb9f0b4c27850a3096e797aada</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -11331,7 +11331,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>09553ce9-1ae1-4156-a6f7-c239654c7847</t>
+          <t>b91a1bc1-abbc-41ae-8f1c-5115ed8c076b</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -11341,7 +11341,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -11354,7 +11354,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>https://www.notion.so/50-09553ce91ae14156a6f7c239654c7847</t>
+          <t>https://www.notion.so/50-b91a1bc1abbc41ae8f1c5115ed8c076b</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -11548,7 +11548,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>b1e72825-b8ab-4bba-a7ec-36a8010b9d53</t>
+          <t>09553ce9-1ae1-4156-a6f7-c239654c7847</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -11558,7 +11558,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -11571,7 +11571,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>https://www.notion.so/51-b1e72825b8ab4bbaa7ec36a8010b9d53</t>
+          <t>https://www.notion.so/51-09553ce91ae14156a6f7c239654c7847</t>
         </is>
       </c>
       <c r="J52" t="inlineStr"/>
@@ -11765,7 +11765,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>c992cc9b-e4a4-42bf-9292-ecbf3d444afb</t>
+          <t>b1e72825-b8ab-4bba-a7ec-36a8010b9d53</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -11775,7 +11775,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -11788,7 +11788,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>https://www.notion.so/52-c992cc9be4a442bf9292ecbf3d444afb</t>
+          <t>https://www.notion.so/52-b1e72825b8ab4bbaa7ec36a8010b9d53</t>
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
@@ -11982,7 +11982,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1f293830-720a-47e6-8684-dc7441d8c647</t>
+          <t>c992cc9b-e4a4-42bf-9292-ecbf3d444afb</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -11992,7 +11992,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -12005,7 +12005,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>https://www.notion.so/53-1f293830720a47e68684dc7441d8c647</t>
+          <t>https://www.notion.so/53-c992cc9be4a442bf9292ecbf3d444afb</t>
         </is>
       </c>
       <c r="J54" t="inlineStr"/>
@@ -12199,7 +12199,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>09c4941f-1337-4ff6-8d2d-fd350249ff4f</t>
+          <t>1f293830-720a-47e6-8684-dc7441d8c647</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -12209,7 +12209,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -12222,7 +12222,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>https://www.notion.so/54-09c4941f13374ff68d2dfd350249ff4f</t>
+          <t>https://www.notion.so/54-1f293830720a47e68684dc7441d8c647</t>
         </is>
       </c>
       <c r="J55" t="inlineStr"/>
@@ -12416,7 +12416,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>13a3ba95-1ecd-47ab-b5a7-8505067eb7f4</t>
+          <t>09c4941f-1337-4ff6-8d2d-fd350249ff4f</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -12426,7 +12426,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -12439,7 +12439,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>https://www.notion.so/55-13a3ba951ecd47abb5a78505067eb7f4</t>
+          <t>https://www.notion.so/55-09c4941f13374ff68d2dfd350249ff4f</t>
         </is>
       </c>
       <c r="J56" t="inlineStr"/>
@@ -12633,7 +12633,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>76c25655-8bdf-4a36-9366-de1af3abbd59</t>
+          <t>13a3ba95-1ecd-47ab-b5a7-8505067eb7f4</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -12643,7 +12643,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -12656,7 +12656,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>https://www.notion.so/56-76c256558bdf4a369366de1af3abbd59</t>
+          <t>https://www.notion.so/56-13a3ba951ecd47abb5a78505067eb7f4</t>
         </is>
       </c>
       <c r="J57" t="inlineStr"/>
@@ -12850,7 +12850,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2d16cd2a-d3f6-4614-a322-95c0ff2e1932</t>
+          <t>76c25655-8bdf-4a36-9366-de1af3abbd59</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -12860,7 +12860,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -12873,7 +12873,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>https://www.notion.so/57-2d16cd2ad3f64614a32295c0ff2e1932</t>
+          <t>https://www.notion.so/57-76c256558bdf4a369366de1af3abbd59</t>
         </is>
       </c>
       <c r="J58" t="inlineStr"/>
@@ -13067,7 +13067,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2b907fc2-cb5f-4e57-b12f-96529f925caa</t>
+          <t>2d16cd2a-d3f6-4614-a322-95c0ff2e1932</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -13077,7 +13077,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -13090,7 +13090,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>https://www.notion.so/58-2b907fc2cb5f4e57b12f96529f925caa</t>
+          <t>https://www.notion.so/58-2d16cd2ad3f64614a32295c0ff2e1932</t>
         </is>
       </c>
       <c r="J59" t="inlineStr"/>
@@ -13284,7 +13284,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>b010dadd-e399-4352-9046-d832559a9b9d</t>
+          <t>2b907fc2-cb5f-4e57-b12f-96529f925caa</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -13294,7 +13294,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -13307,7 +13307,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>https://www.notion.so/59-b010dadde39943529046d832559a9b9d</t>
+          <t>https://www.notion.so/59-2b907fc2cb5f4e57b12f96529f925caa</t>
         </is>
       </c>
       <c r="J60" t="inlineStr"/>
@@ -13501,7 +13501,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1e19c8a8-2d9a-4e80-9ca0-a34294dd3f99</t>
+          <t>b010dadd-e399-4352-9046-d832559a9b9d</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -13511,7 +13511,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -13524,7 +13524,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>https://www.notion.so/60-1e19c8a82d9a4e809ca0a34294dd3f99</t>
+          <t>https://www.notion.so/60-b010dadde39943529046d832559a9b9d</t>
         </is>
       </c>
       <c r="J61" t="inlineStr"/>
@@ -13718,7 +13718,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>9e8c94d1-45de-4a0c-8bb4-5a3ef8033f59</t>
+          <t>1e19c8a8-2d9a-4e80-9ca0-a34294dd3f99</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -13728,7 +13728,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -13741,7 +13741,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>https://www.notion.so/61-9e8c94d145de4a0c8bb45a3ef8033f59</t>
+          <t>https://www.notion.so/61-1e19c8a82d9a4e809ca0a34294dd3f99</t>
         </is>
       </c>
       <c r="J62" t="inlineStr"/>
@@ -13935,7 +13935,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>e3af674b-0930-46bb-9565-45f139657c05</t>
+          <t>9e8c94d1-45de-4a0c-8bb4-5a3ef8033f59</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -13945,7 +13945,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -13958,7 +13958,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>https://www.notion.so/62-e3af674b093046bb956545f139657c05</t>
+          <t>https://www.notion.so/62-9e8c94d145de4a0c8bb45a3ef8033f59</t>
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
@@ -14152,7 +14152,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5a5cefea-cbd8-41cd-b5d0-dcd547274de9</t>
+          <t>e3af674b-0930-46bb-9565-45f139657c05</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -14162,7 +14162,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -14175,7 +14175,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>https://www.notion.so/63-5a5cefeacbd841cdb5d0dcd547274de9</t>
+          <t>https://www.notion.so/63-e3af674b093046bb956545f139657c05</t>
         </is>
       </c>
       <c r="J64" t="inlineStr"/>
@@ -14369,7 +14369,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>e233f83e-f2c2-459e-9f08-05051fbdc257</t>
+          <t>5a5cefea-cbd8-41cd-b5d0-dcd547274de9</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -14379,7 +14379,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -14392,7 +14392,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>https://www.notion.so/64-e233f83ef2c2459e9f0805051fbdc257</t>
+          <t>https://www.notion.so/64-5a5cefeacbd841cdb5d0dcd547274de9</t>
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
@@ -14586,7 +14586,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>58142be4-00ee-435f-ac0a-dd0be7b6bbeb</t>
+          <t>e233f83e-f2c2-459e-9f08-05051fbdc257</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -14596,7 +14596,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -14609,7 +14609,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>https://www.notion.so/65-58142be400ee435fac0add0be7b6bbeb</t>
+          <t>https://www.notion.so/65-e233f83ef2c2459e9f0805051fbdc257</t>
         </is>
       </c>
       <c r="J66" t="inlineStr"/>
@@ -14803,7 +14803,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>427b861d-7917-4e7f-8db6-7da3b3cf80a6</t>
+          <t>58142be4-00ee-435f-ac0a-dd0be7b6bbeb</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -14813,7 +14813,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -14826,7 +14826,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>https://www.notion.so/66-427b861d79174e7f8db67da3b3cf80a6</t>
+          <t>https://www.notion.so/66-58142be400ee435fac0add0be7b6bbeb</t>
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
@@ -15020,7 +15020,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>11fb8060-280e-45f4-867c-fe5bd15411a0</t>
+          <t>427b861d-7917-4e7f-8db6-7da3b3cf80a6</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -15030,7 +15030,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -15043,7 +15043,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>https://www.notion.so/67-11fb8060280e45f4867cfe5bd15411a0</t>
+          <t>https://www.notion.so/67-427b861d79174e7f8db67da3b3cf80a6</t>
         </is>
       </c>
       <c r="J68" t="inlineStr"/>
@@ -15237,7 +15237,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8122a3bb-6764-4ab7-b787-84f3f2ca87ee</t>
+          <t>11fb8060-280e-45f4-867c-fe5bd15411a0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -15247,7 +15247,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -15260,7 +15260,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>https://www.notion.so/68-8122a3bb67644ab7b78784f3f2ca87ee</t>
+          <t>https://www.notion.so/68-11fb8060280e45f4867cfe5bd15411a0</t>
         </is>
       </c>
       <c r="J69" t="inlineStr"/>
@@ -15454,7 +15454,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>b4c2d49b-afb7-407b-bde0-f0f73f20353a</t>
+          <t>8122a3bb-6764-4ab7-b787-84f3f2ca87ee</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -15464,7 +15464,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -15477,7 +15477,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>https://www.notion.so/69-b4c2d49bafb7407bbde0f0f73f20353a</t>
+          <t>https://www.notion.so/69-8122a3bb67644ab7b78784f3f2ca87ee</t>
         </is>
       </c>
       <c r="J70" t="inlineStr"/>
@@ -15671,7 +15671,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>041df600-3403-42b8-bd0c-a5d61e0f2214</t>
+          <t>b4c2d49b-afb7-407b-bde0-f0f73f20353a</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -15681,7 +15681,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
@@ -15694,7 +15694,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>https://www.notion.so/70-041df600340342b8bd0ca5d61e0f2214</t>
+          <t>https://www.notion.so/70-b4c2d49bafb7407bbde0f0f73f20353a</t>
         </is>
       </c>
       <c r="J71" t="inlineStr"/>
@@ -15888,7 +15888,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>35d891f2-1f92-42ed-b02a-0ac30333cedf</t>
+          <t>041df600-3403-42b8-bd0c-a5d61e0f2214</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -15898,7 +15898,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -15911,7 +15911,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>https://www.notion.so/71-35d891f21f9242edb02a0ac30333cedf</t>
+          <t>https://www.notion.so/71-041df600340342b8bd0ca5d61e0f2214</t>
         </is>
       </c>
       <c r="J72" t="inlineStr"/>
@@ -16105,7 +16105,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5d77ed79-565d-46c2-bc6a-2535cf4837ae</t>
+          <t>35d891f2-1f92-42ed-b02a-0ac30333cedf</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -16115,7 +16115,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -16128,7 +16128,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>https://www.notion.so/72-5d77ed79565d46c2bc6a2535cf4837ae</t>
+          <t>https://www.notion.so/72-35d891f21f9242edb02a0ac30333cedf</t>
         </is>
       </c>
       <c r="J73" t="inlineStr"/>
@@ -16322,7 +16322,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>e6730d11-380a-41bb-a8d5-8d3c50bd9222</t>
+          <t>5d77ed79-565d-46c2-bc6a-2535cf4837ae</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -16332,7 +16332,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
@@ -16345,7 +16345,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>https://www.notion.so/73-e6730d11380a41bba8d58d3c50bd9222</t>
+          <t>https://www.notion.so/73-5d77ed79565d46c2bc6a2535cf4837ae</t>
         </is>
       </c>
       <c r="J74" t="inlineStr"/>
@@ -16539,7 +16539,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>f1f89d36-3dfc-47f0-adc4-b7f4944a11b4</t>
+          <t>e6730d11-380a-41bb-a8d5-8d3c50bd9222</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -16549,7 +16549,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -16562,7 +16562,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>https://www.notion.so/74-f1f89d363dfc47f0adc4b7f4944a11b4</t>
+          <t>https://www.notion.so/74-e6730d11380a41bba8d58d3c50bd9222</t>
         </is>
       </c>
       <c r="J75" t="inlineStr"/>
@@ -16756,7 +16756,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>4163582a-d393-4443-9921-faee57f55b8a</t>
+          <t>f1f89d36-3dfc-47f0-adc4-b7f4944a11b4</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -16766,7 +16766,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -16779,7 +16779,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>https://www.notion.so/75-4163582ad39344439921faee57f55b8a</t>
+          <t>https://www.notion.so/75-f1f89d363dfc47f0adc4b7f4944a11b4</t>
         </is>
       </c>
       <c r="J76" t="inlineStr"/>
@@ -16973,7 +16973,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>bedc4c40-3289-481a-a093-d1cd90e5032d</t>
+          <t>4163582a-d393-4443-9921-faee57f55b8a</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -16983,7 +16983,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
@@ -16996,7 +16996,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>https://www.notion.so/76-bedc4c403289481aa093d1cd90e5032d</t>
+          <t>https://www.notion.so/76-4163582ad39344439921faee57f55b8a</t>
         </is>
       </c>
       <c r="J77" t="inlineStr"/>
@@ -17190,7 +17190,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>06a4d1f1-edf0-493f-ab60-8a5a0c455d04</t>
+          <t>bedc4c40-3289-481a-a093-d1cd90e5032d</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -17200,7 +17200,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -17213,7 +17213,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>https://www.notion.so/77-06a4d1f1edf0493fab608a5a0c455d04</t>
+          <t>https://www.notion.so/77-bedc4c403289481aa093d1cd90e5032d</t>
         </is>
       </c>
       <c r="J78" t="inlineStr"/>
@@ -17407,7 +17407,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>b2b51a2a-2ddf-4a49-b11a-7ffe4deed937</t>
+          <t>06a4d1f1-edf0-493f-ab60-8a5a0c455d04</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -17417,7 +17417,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -17430,7 +17430,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>https://www.notion.so/78-b2b51a2a2ddf4a49b11a7ffe4deed937</t>
+          <t>https://www.notion.so/78-06a4d1f1edf0493fab608a5a0c455d04</t>
         </is>
       </c>
       <c r="J79" t="inlineStr"/>
@@ -17624,7 +17624,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>496173c5-f40f-43c0-ae34-76c5279256f8</t>
+          <t>b2b51a2a-2ddf-4a49-b11a-7ffe4deed937</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -17634,7 +17634,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -17647,7 +17647,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>https://www.notion.so/79-496173c5f40f43c0ae3476c5279256f8</t>
+          <t>https://www.notion.so/79-b2b51a2a2ddf4a49b11a7ffe4deed937</t>
         </is>
       </c>
       <c r="J80" t="inlineStr"/>
@@ -17841,7 +17841,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>d5e63696-3120-4f11-93e9-85e1408862a0</t>
+          <t>496173c5-f40f-43c0-ae34-76c5279256f8</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -17851,7 +17851,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -17864,7 +17864,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>https://www.notion.so/80-d5e6369631204f1193e985e1408862a0</t>
+          <t>https://www.notion.so/80-496173c5f40f43c0ae3476c5279256f8</t>
         </is>
       </c>
       <c r="J81" t="inlineStr"/>
@@ -18058,7 +18058,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7cad04af-538e-4d13-a195-a2aef6732c19</t>
+          <t>d5e63696-3120-4f11-93e9-85e1408862a0</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -18068,7 +18068,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E82" t="inlineStr"/>
@@ -18081,7 +18081,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>https://www.notion.so/81-7cad04af538e4d13a195a2aef6732c19</t>
+          <t>https://www.notion.so/81-d5e6369631204f1193e985e1408862a0</t>
         </is>
       </c>
       <c r="J82" t="inlineStr"/>
@@ -18275,7 +18275,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>05c57336-b708-4d9b-8e6a-89b7b95be6b7</t>
+          <t>7cad04af-538e-4d13-a195-a2aef6732c19</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -18285,7 +18285,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E83" t="inlineStr"/>
@@ -18298,7 +18298,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>https://www.notion.so/82-05c57336b7084d9b8e6a89b7b95be6b7</t>
+          <t>https://www.notion.so/82-7cad04af538e4d13a195a2aef6732c19</t>
         </is>
       </c>
       <c r="J83" t="inlineStr"/>
@@ -18492,7 +18492,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>843c0f3c-8123-433b-88b3-97d27986224f</t>
+          <t>05c57336-b708-4d9b-8e6a-89b7b95be6b7</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -18502,7 +18502,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2024-07-04T09:48:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -18515,7 +18515,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>https://www.notion.so/83-843c0f3c8123433b88b397d27986224f</t>
+          <t>https://www.notion.so/83-05c57336b7084d9b8e6a89b7b95be6b7</t>
         </is>
       </c>
       <c r="J84" t="inlineStr"/>
@@ -18709,7 +18709,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>862f1a06-2204-4195-90ec-cac4dc9face7</t>
+          <t>843c0f3c-8123-433b-88b3-97d27986224f</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -18719,7 +18719,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2024-07-04T09:44:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -18732,7 +18732,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>https://www.notion.so/84-862f1a062204419590eccac4dc9face7</t>
+          <t>https://www.notion.so/84-843c0f3c8123433b88b397d27986224f</t>
         </is>
       </c>
       <c r="J85" t="inlineStr"/>
@@ -18926,7 +18926,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>5a20033c-7b76-441e-a043-11a24bafe817</t>
+          <t>862f1a06-2204-4195-90ec-cac4dc9face7</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -18936,7 +18936,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2024-07-04T09:44:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -18949,7 +18949,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>https://www.notion.so/85-5a20033c7b76441ea04311a24bafe817</t>
+          <t>https://www.notion.so/85-862f1a062204419590eccac4dc9face7</t>
         </is>
       </c>
       <c r="J86" t="inlineStr"/>
@@ -19143,7 +19143,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>4bb0f678-a35b-4cdf-aa60-42d5723edb56</t>
+          <t>5a20033c-7b76-441e-a043-11a24bafe817</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -19153,7 +19153,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2024-07-04T09:44:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
@@ -19166,7 +19166,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>https://www.notion.so/86-4bb0f678a35b4cdfaa6042d5723edb56</t>
+          <t>https://www.notion.so/86-5a20033c7b76441ea04311a24bafe817</t>
         </is>
       </c>
       <c r="J87" t="inlineStr"/>
@@ -19360,7 +19360,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8e1ea00e-bd3f-4195-917e-a4f95caeca3e</t>
+          <t>4bb0f678-a35b-4cdf-aa60-42d5723edb56</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -19370,7 +19370,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2024-07-04T09:44:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
@@ -19383,7 +19383,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>https://www.notion.so/87-8e1ea00ebd3f4195917ea4f95caeca3e</t>
+          <t>https://www.notion.so/87-4bb0f678a35b4cdfaa6042d5723edb56</t>
         </is>
       </c>
       <c r="J88" t="inlineStr"/>
@@ -19577,7 +19577,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>26a7f7ee-02ed-4fb1-83c8-ec84258e73c1</t>
+          <t>8e1ea00e-bd3f-4195-917e-a4f95caeca3e</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -19587,7 +19587,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2024-07-04T09:44:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -19600,7 +19600,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>https://www.notion.so/88-26a7f7ee02ed4fb183c8ec84258e73c1</t>
+          <t>https://www.notion.so/88-8e1ea00ebd3f4195917ea4f95caeca3e</t>
         </is>
       </c>
       <c r="J89" t="inlineStr"/>
@@ -19794,7 +19794,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>49be2302-44bd-4319-9dfd-ba3efecee188</t>
+          <t>26a7f7ee-02ed-4fb1-83c8-ec84258e73c1</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -19804,7 +19804,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2024-07-04T09:44:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -19817,7 +19817,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>https://www.notion.so/89-49be230244bd43199dfdba3efecee188</t>
+          <t>https://www.notion.so/89-26a7f7ee02ed4fb183c8ec84258e73c1</t>
         </is>
       </c>
       <c r="J90" t="inlineStr"/>
@@ -20011,17 +20011,17 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>e3d0e7f2-3a0f-4b21-854d-275f27645ccb</t>
+          <t>49be2302-44bd-4319-9dfd-ba3efecee188</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2024-06-24T17:11:00.000Z</t>
+          <t>2024-06-24T17:12:00.000Z</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -20034,7 +20034,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>https://www.notion.so/90-e3d0e7f23a0f4b21854d275f27645ccb</t>
+          <t>https://www.notion.so/90-49be230244bd43199dfdba3efecee188</t>
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
@@ -20228,7 +20228,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>b39a1a5d-b3d2-4e1f-a621-4c7ef48fbd42</t>
+          <t>e3d0e7f2-3a0f-4b21-854d-275f27645ccb</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -20238,7 +20238,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E92" t="inlineStr"/>
@@ -20251,7 +20251,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>https://www.notion.so/91-b39a1a5db3d24e1fa6214c7ef48fbd42</t>
+          <t>https://www.notion.so/91-e3d0e7f23a0f4b21854d275f27645ccb</t>
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
@@ -20445,7 +20445,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>493985da-d6ad-4058-8b64-843eee3d8f2d</t>
+          <t>b39a1a5d-b3d2-4e1f-a621-4c7ef48fbd42</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -20455,7 +20455,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -20468,7 +20468,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>https://www.notion.so/92-493985dad6ad40588b64843eee3d8f2d</t>
+          <t>https://www.notion.so/92-b39a1a5db3d24e1fa6214c7ef48fbd42</t>
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
@@ -20662,7 +20662,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>42672126-8639-4fad-a41f-20bcff3ce428</t>
+          <t>493985da-d6ad-4058-8b64-843eee3d8f2d</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -20672,7 +20672,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:11:00.000Z</t>
         </is>
       </c>
       <c r="E94" t="inlineStr"/>
@@ -20685,7 +20685,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>https://www.notion.so/93-4267212686394fada41f20bcff3ce428</t>
+          <t>https://www.notion.so/93-493985dad6ad40588b64843eee3d8f2d</t>
         </is>
       </c>
       <c r="J94" t="inlineStr"/>
@@ -20879,7 +20879,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>dac6c1eb-aeef-4eac-bee0-c1fde79f21b1</t>
+          <t>42672126-8639-4fad-a41f-20bcff3ce428</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -20889,7 +20889,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
@@ -20902,7 +20902,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>https://www.notion.so/94-dac6c1ebaeef4eacbee0c1fde79f21b1</t>
+          <t>https://www.notion.so/94-4267212686394fada41f20bcff3ce428</t>
         </is>
       </c>
       <c r="J95" t="inlineStr"/>
@@ -21096,7 +21096,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>0c9dfa61-f5cc-4fb7-916d-03c4f3257b2c</t>
+          <t>dac6c1eb-aeef-4eac-bee0-c1fde79f21b1</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -21106,7 +21106,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E96" t="inlineStr"/>
@@ -21119,7 +21119,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>https://www.notion.so/95-0c9dfa61f5cc4fb7916d03c4f3257b2c</t>
+          <t>https://www.notion.so/95-dac6c1ebaeef4eacbee0c1fde79f21b1</t>
         </is>
       </c>
       <c r="J96" t="inlineStr"/>
@@ -21313,7 +21313,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>42241cf4-f792-4387-80e7-82225df7215f</t>
+          <t>0c9dfa61-f5cc-4fb7-916d-03c4f3257b2c</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -21323,7 +21323,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
@@ -21336,7 +21336,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>https://www.notion.so/96-42241cf4f792438780e782225df7215f</t>
+          <t>https://www.notion.so/96-0c9dfa61f5cc4fb7916d03c4f3257b2c</t>
         </is>
       </c>
       <c r="J97" t="inlineStr"/>
@@ -21530,7 +21530,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>d6f8d60a-4b22-4c98-be85-095455a283da</t>
+          <t>42241cf4-f792-4387-80e7-82225df7215f</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -21540,7 +21540,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -21553,7 +21553,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>https://www.notion.so/97-d6f8d60a4b224c98be85095455a283da</t>
+          <t>https://www.notion.so/97-42241cf4f792438780e782225df7215f</t>
         </is>
       </c>
       <c r="J98" t="inlineStr"/>
@@ -21747,7 +21747,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>1c4ce883-3380-4268-89d2-0cb7795e63ba</t>
+          <t>d6f8d60a-4b22-4c98-be85-095455a283da</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -21757,7 +21757,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -21770,7 +21770,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>https://www.notion.so/98-1c4ce8833380426889d20cb7795e63ba</t>
+          <t>https://www.notion.so/98-d6f8d60a4b224c98be85095455a283da</t>
         </is>
       </c>
       <c r="J99" t="inlineStr"/>
@@ -21964,7 +21964,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>80a7d602-7106-441a-b801-b93fdaa517b1</t>
+          <t>1c4ce883-3380-4268-89d2-0cb7795e63ba</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -21974,7 +21974,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E100" t="inlineStr"/>
@@ -21987,7 +21987,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>https://www.notion.so/99-80a7d6027106441ab801b93fdaa517b1</t>
+          <t>https://www.notion.so/99-1c4ce8833380426889d20cb7795e63ba</t>
         </is>
       </c>
       <c r="J100" t="inlineStr"/>
@@ -22181,7 +22181,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>a0b354b1-c1ed-42e6-9cdf-3648200eb567</t>
+          <t>80a7d602-7106-441a-b801-b93fdaa517b1</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -22191,7 +22191,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>
@@ -22204,7 +22204,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>https://www.notion.so/100-a0b354b1c1ed42e69cdf3648200eb567</t>
+          <t>https://www.notion.so/100-80a7d6027106441ab801b93fdaa517b1</t>
         </is>
       </c>
       <c r="J101" t="inlineStr"/>
@@ -22398,7 +22398,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>ffd66113-90bc-4b60-a2a0-35b23d0683f6</t>
+          <t>a0b354b1-c1ed-42e6-9cdf-3648200eb567</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -22408,7 +22408,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E102" t="inlineStr"/>
@@ -22421,7 +22421,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>https://www.notion.so/101-ffd6611390bc4b60a2a035b23d0683f6</t>
+          <t>https://www.notion.so/101-a0b354b1c1ed42e69cdf3648200eb567</t>
         </is>
       </c>
       <c r="J102" t="inlineStr"/>
@@ -22615,7 +22615,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>1a76f663-e849-4e18-90f6-4e2a6dde02fc</t>
+          <t>ffd66113-90bc-4b60-a2a0-35b23d0683f6</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -22625,7 +22625,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E103" t="inlineStr"/>
@@ -22638,7 +22638,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>https://www.notion.so/102-1a76f663e8494e1890f64e2a6dde02fc</t>
+          <t>https://www.notion.so/102-ffd6611390bc4b60a2a035b23d0683f6</t>
         </is>
       </c>
       <c r="J103" t="inlineStr"/>
@@ -22832,7 +22832,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>83559fb8-d2fe-48c8-8cdc-cae71e18a107</t>
+          <t>1a76f663-e849-4e18-90f6-4e2a6dde02fc</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -22842,7 +22842,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E104" t="inlineStr"/>
@@ -22855,7 +22855,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>https://www.notion.so/103-83559fb8d2fe48c88cdccae71e18a107</t>
+          <t>https://www.notion.so/103-1a76f663e8494e1890f64e2a6dde02fc</t>
         </is>
       </c>
       <c r="J104" t="inlineStr"/>
@@ -22962,7 +22962,7 @@
         </is>
       </c>
       <c r="AG104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH104" t="inlineStr">
         <is>
@@ -23049,7 +23049,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>33d50674-8474-41c5-8386-a8ad4c4ab5de</t>
+          <t>83559fb8-d2fe-48c8-8cdc-cae71e18a107</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -23059,7 +23059,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
@@ -23072,7 +23072,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>https://www.notion.so/104-33d50674847441c58386a8ad4c4ab5de</t>
+          <t>https://www.notion.so/104-83559fb8d2fe48c88cdccae71e18a107</t>
         </is>
       </c>
       <c r="J105" t="inlineStr"/>
@@ -23266,7 +23266,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>37128e53-b773-4ea2-96bf-972affc6cc26</t>
+          <t>33d50674-8474-41c5-8386-a8ad4c4ab5de</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -23276,7 +23276,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
@@ -23289,7 +23289,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>https://www.notion.so/105-37128e53b7734ea296bf972affc6cc26</t>
+          <t>https://www.notion.so/105-33d50674847441c58386a8ad4c4ab5de</t>
         </is>
       </c>
       <c r="J106" t="inlineStr"/>
@@ -23483,7 +23483,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>7253fb5a-bf33-4ccd-8fd0-91f4b9969ef6</t>
+          <t>37128e53-b773-4ea2-96bf-972affc6cc26</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -23493,7 +23493,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E107" t="inlineStr"/>
@@ -23506,7 +23506,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>https://www.notion.so/106-7253fb5abf334ccd8fd091f4b9969ef6</t>
+          <t>https://www.notion.so/106-37128e53b7734ea296bf972affc6cc26</t>
         </is>
       </c>
       <c r="J107" t="inlineStr"/>
@@ -23700,7 +23700,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>e929925c-ebe4-4ca8-b41c-3de560b2837c</t>
+          <t>7253fb5a-bf33-4ccd-8fd0-91f4b9969ef6</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -23710,7 +23710,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E108" t="inlineStr"/>
@@ -23723,7 +23723,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>https://www.notion.so/107-e929925cebe44ca8b41c3de560b2837c</t>
+          <t>https://www.notion.so/107-7253fb5abf334ccd8fd091f4b9969ef6</t>
         </is>
       </c>
       <c r="J108" t="inlineStr"/>
@@ -23917,7 +23917,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>9dab23a5-43ce-4360-ac1c-03a9c3e6ed32</t>
+          <t>e929925c-ebe4-4ca8-b41c-3de560b2837c</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -23927,7 +23927,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
@@ -23940,7 +23940,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>https://www.notion.so/108-9dab23a543ce4360ac1c03a9c3e6ed32</t>
+          <t>https://www.notion.so/108-e929925cebe44ca8b41c3de560b2837c</t>
         </is>
       </c>
       <c r="J109" t="inlineStr"/>
@@ -24134,7 +24134,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>6c863667-9f48-402b-8e54-f7a90e88236f</t>
+          <t>9dab23a5-43ce-4360-ac1c-03a9c3e6ed32</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -24144,7 +24144,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E110" t="inlineStr"/>
@@ -24157,7 +24157,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>https://www.notion.so/109-6c8636679f48402b8e54f7a90e88236f</t>
+          <t>https://www.notion.so/109-9dab23a543ce4360ac1c03a9c3e6ed32</t>
         </is>
       </c>
       <c r="J110" t="inlineStr"/>
@@ -24351,7 +24351,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>4d129591-2cfa-4125-9a26-bd0482773b60</t>
+          <t>6c863667-9f48-402b-8e54-f7a90e88236f</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -24361,7 +24361,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -24374,7 +24374,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>https://www.notion.so/110-4d1295912cfa41259a26bd0482773b60</t>
+          <t>https://www.notion.so/110-6c8636679f48402b8e54f7a90e88236f</t>
         </is>
       </c>
       <c r="J111" t="inlineStr"/>
@@ -24568,7 +24568,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>24fc52cb-6fb1-48a9-9009-773c42ccef04</t>
+          <t>4d129591-2cfa-4125-9a26-bd0482773b60</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -24578,7 +24578,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E112" t="inlineStr"/>
@@ -24591,7 +24591,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>https://www.notion.so/111-24fc52cb6fb148a99009773c42ccef04</t>
+          <t>https://www.notion.so/111-4d1295912cfa41259a26bd0482773b60</t>
         </is>
       </c>
       <c r="J112" t="inlineStr"/>
@@ -24785,7 +24785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2e8f6b21-caba-4b14-8110-c0ed9b2f93c8</t>
+          <t>24fc52cb-6fb1-48a9-9009-773c42ccef04</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -24795,7 +24795,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
@@ -24808,7 +24808,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>https://www.notion.so/112-2e8f6b21caba4b148110c0ed9b2f93c8</t>
+          <t>https://www.notion.so/112-24fc52cb6fb148a99009773c42ccef04</t>
         </is>
       </c>
       <c r="J113" t="inlineStr"/>
@@ -25002,7 +25002,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>efabbe44-5db8-4011-bb36-47628eaa630f</t>
+          <t>2e8f6b21-caba-4b14-8110-c0ed9b2f93c8</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -25012,7 +25012,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E114" t="inlineStr"/>
@@ -25025,7 +25025,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>https://www.notion.so/113-efabbe445db84011bb3647628eaa630f</t>
+          <t>https://www.notion.so/113-2e8f6b21caba4b148110c0ed9b2f93c8</t>
         </is>
       </c>
       <c r="J114" t="inlineStr"/>
@@ -25219,7 +25219,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>06f63b1c-cbf4-4c5f-a3d1-29d7f16153a0</t>
+          <t>efabbe44-5db8-4011-bb36-47628eaa630f</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -25229,7 +25229,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E115" t="inlineStr"/>
@@ -25242,7 +25242,7 @@
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>https://www.notion.so/114-06f63b1ccbf44c5fa3d129d7f16153a0</t>
+          <t>https://www.notion.so/114-efabbe445db84011bb3647628eaa630f</t>
         </is>
       </c>
       <c r="J115" t="inlineStr"/>
@@ -25436,7 +25436,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>8b90e615-6115-4700-ba83-4432306a036c</t>
+          <t>06f63b1c-cbf4-4c5f-a3d1-29d7f16153a0</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -25446,7 +25446,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E116" t="inlineStr"/>
@@ -25459,7 +25459,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>https://www.notion.so/115-8b90e61561154700ba834432306a036c</t>
+          <t>https://www.notion.so/115-06f63b1ccbf44c5fa3d129d7f16153a0</t>
         </is>
       </c>
       <c r="J116" t="inlineStr"/>
@@ -25653,7 +25653,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>a19e566b-7859-4527-be9a-072bd8c05390</t>
+          <t>8b90e615-6115-4700-ba83-4432306a036c</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -25663,7 +25663,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E117" t="inlineStr"/>
@@ -25676,7 +25676,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>https://www.notion.so/116-a19e566b78594527be9a072bd8c05390</t>
+          <t>https://www.notion.so/116-8b90e61561154700ba834432306a036c</t>
         </is>
       </c>
       <c r="J117" t="inlineStr"/>
@@ -25870,7 +25870,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>001d4caf-f4de-4678-b0f0-761c92275cf7</t>
+          <t>a19e566b-7859-4527-be9a-072bd8c05390</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -25880,7 +25880,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E118" t="inlineStr"/>
@@ -25893,7 +25893,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>https://www.notion.so/117-001d4caff4de4678b0f0761c92275cf7</t>
+          <t>https://www.notion.so/117-a19e566b78594527be9a072bd8c05390</t>
         </is>
       </c>
       <c r="J118" t="inlineStr"/>
@@ -26087,7 +26087,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>d5f56ef4-f178-40b4-b16f-5c14ffe31e13</t>
+          <t>001d4caf-f4de-4678-b0f0-761c92275cf7</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -26097,7 +26097,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E119" t="inlineStr"/>
@@ -26110,7 +26110,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>https://www.notion.so/118-d5f56ef4f17840b4b16f5c14ffe31e13</t>
+          <t>https://www.notion.so/118-001d4caff4de4678b0f0761c92275cf7</t>
         </is>
       </c>
       <c r="J119" t="inlineStr"/>
@@ -26304,7 +26304,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>e65b3e23-103d-478e-801a-bf7777c8f2eb</t>
+          <t>d5f56ef4-f178-40b4-b16f-5c14ffe31e13</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -26314,7 +26314,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E120" t="inlineStr"/>
@@ -26327,7 +26327,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>https://www.notion.so/119-e65b3e23103d478e801abf7777c8f2eb</t>
+          <t>https://www.notion.so/119-d5f56ef4f17840b4b16f5c14ffe31e13</t>
         </is>
       </c>
       <c r="J120" t="inlineStr"/>
@@ -26521,7 +26521,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>caaed0bc-bfa5-4d55-8b43-ab30c77c1785</t>
+          <t>e65b3e23-103d-478e-801a-bf7777c8f2eb</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -26531,7 +26531,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E121" t="inlineStr"/>
@@ -26544,7 +26544,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>https://www.notion.so/120-caaed0bcbfa54d558b43ab30c77c1785</t>
+          <t>https://www.notion.so/120-e65b3e23103d478e801abf7777c8f2eb</t>
         </is>
       </c>
       <c r="J121" t="inlineStr"/>
@@ -26738,7 +26738,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>822dc4c7-461a-4244-b0c0-4864e890788b</t>
+          <t>caaed0bc-bfa5-4d55-8b43-ab30c77c1785</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -26748,7 +26748,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E122" t="inlineStr"/>
@@ -26761,7 +26761,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>https://www.notion.so/121-822dc4c7461a4244b0c04864e890788b</t>
+          <t>https://www.notion.so/121-caaed0bcbfa54d558b43ab30c77c1785</t>
         </is>
       </c>
       <c r="J122" t="inlineStr"/>
@@ -26955,7 +26955,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>9dc50016-75f8-4ebb-becc-f7c19023df88</t>
+          <t>822dc4c7-461a-4244-b0c0-4864e890788b</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -26965,7 +26965,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E123" t="inlineStr"/>
@@ -26978,7 +26978,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>https://www.notion.so/122-9dc5001675f84ebbbeccf7c19023df88</t>
+          <t>https://www.notion.so/122-822dc4c7461a4244b0c04864e890788b</t>
         </is>
       </c>
       <c r="J123" t="inlineStr"/>
@@ -27172,7 +27172,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>46b797ad-bc4f-4f9e-8fc1-10fb45a779b0</t>
+          <t>9dc50016-75f8-4ebb-becc-f7c19023df88</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -27182,7 +27182,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E124" t="inlineStr"/>
@@ -27195,7 +27195,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>https://www.notion.so/123-46b797adbc4f4f9e8fc110fb45a779b0</t>
+          <t>https://www.notion.so/123-9dc5001675f84ebbbeccf7c19023df88</t>
         </is>
       </c>
       <c r="J124" t="inlineStr"/>
@@ -27389,7 +27389,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>60f8a8d9-03b1-4152-83a7-76617f1fae5f</t>
+          <t>46b797ad-bc4f-4f9e-8fc1-10fb45a779b0</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -27399,7 +27399,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E125" t="inlineStr"/>
@@ -27412,7 +27412,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>https://www.notion.so/124-60f8a8d903b1415283a776617f1fae5f</t>
+          <t>https://www.notion.so/124-46b797adbc4f4f9e8fc110fb45a779b0</t>
         </is>
       </c>
       <c r="J125" t="inlineStr"/>
@@ -27606,7 +27606,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>bd97bf52-0298-4456-840b-fc17fd7cc090</t>
+          <t>60f8a8d9-03b1-4152-83a7-76617f1fae5f</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -27616,7 +27616,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E126" t="inlineStr"/>
@@ -27629,7 +27629,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>https://www.notion.so/125-bd97bf5202984456840bfc17fd7cc090</t>
+          <t>https://www.notion.so/125-60f8a8d903b1415283a776617f1fae5f</t>
         </is>
       </c>
       <c r="J126" t="inlineStr"/>
@@ -27823,7 +27823,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>e9eab0ae-4c99-4f20-83fc-0413a44eef94</t>
+          <t>bd97bf52-0298-4456-840b-fc17fd7cc090</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -27833,7 +27833,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E127" t="inlineStr"/>
@@ -27846,7 +27846,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>https://www.notion.so/126-e9eab0ae4c994f2083fc0413a44eef94</t>
+          <t>https://www.notion.so/126-bd97bf5202984456840bfc17fd7cc090</t>
         </is>
       </c>
       <c r="J127" t="inlineStr"/>
@@ -28040,7 +28040,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>1fd0bde0-9f87-405a-9030-94f43b6bc03f</t>
+          <t>e9eab0ae-4c99-4f20-83fc-0413a44eef94</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -28050,7 +28050,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2024-07-04T09:45:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E128" t="inlineStr"/>
@@ -28063,7 +28063,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>https://www.notion.so/127-1fd0bde09f87405a903094f43b6bc03f</t>
+          <t>https://www.notion.so/127-e9eab0ae4c994f2083fc0413a44eef94</t>
         </is>
       </c>
       <c r="J128" t="inlineStr"/>
@@ -28257,7 +28257,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>451bd443-b279-4077-906c-83cd770bc69c</t>
+          <t>1fd0bde0-9f87-405a-9030-94f43b6bc03f</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -28267,7 +28267,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E129" t="inlineStr"/>
@@ -28280,7 +28280,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>https://www.notion.so/128-451bd443b2794077906c83cd770bc69c</t>
+          <t>https://www.notion.so/128-1fd0bde09f87405a903094f43b6bc03f</t>
         </is>
       </c>
       <c r="J129" t="inlineStr"/>
@@ -28474,7 +28474,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>e834216e-5a34-4f07-8fbd-ca240ac98d06</t>
+          <t>451bd443-b279-4077-906c-83cd770bc69c</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -28484,7 +28484,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E130" t="inlineStr"/>
@@ -28497,7 +28497,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>https://www.notion.so/129-e834216e5a344f078fbdca240ac98d06</t>
+          <t>https://www.notion.so/129-451bd443b2794077906c83cd770bc69c</t>
         </is>
       </c>
       <c r="J130" t="inlineStr"/>
@@ -28691,7 +28691,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>f06b3d94-a638-4428-86ad-50c833ddcd28</t>
+          <t>e834216e-5a34-4f07-8fbd-ca240ac98d06</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -28701,7 +28701,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E131" t="inlineStr"/>
@@ -28714,7 +28714,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>https://www.notion.so/130-f06b3d94a638442886ad50c833ddcd28</t>
+          <t>https://www.notion.so/130-e834216e5a344f078fbdca240ac98d06</t>
         </is>
       </c>
       <c r="J131" t="inlineStr"/>
@@ -28908,7 +28908,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>9e02ba25-75bb-4b31-9f89-87b23344eb27</t>
+          <t>f06b3d94-a638-4428-86ad-50c833ddcd28</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -28918,7 +28918,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E132" t="inlineStr"/>
@@ -28931,7 +28931,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>https://www.notion.so/131-9e02ba2575bb4b319f8987b23344eb27</t>
+          <t>https://www.notion.so/131-f06b3d94a638442886ad50c833ddcd28</t>
         </is>
       </c>
       <c r="J132" t="inlineStr"/>
@@ -29125,7 +29125,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>fcbc1dcc-f4d6-46b4-a297-d9ca776b5fc2</t>
+          <t>9e02ba25-75bb-4b31-9f89-87b23344eb27</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -29135,7 +29135,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E133" t="inlineStr"/>
@@ -29148,7 +29148,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>https://www.notion.so/132-fcbc1dccf4d646b4a297d9ca776b5fc2</t>
+          <t>https://www.notion.so/132-9e02ba2575bb4b319f8987b23344eb27</t>
         </is>
       </c>
       <c r="J133" t="inlineStr"/>
@@ -29342,7 +29342,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>afb8c925-ce16-4258-898b-9c4e9a557d0d</t>
+          <t>fcbc1dcc-f4d6-46b4-a297-d9ca776b5fc2</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -29352,7 +29352,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E134" t="inlineStr"/>
@@ -29365,7 +29365,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>https://www.notion.so/133-afb8c925ce164258898b9c4e9a557d0d</t>
+          <t>https://www.notion.so/133-fcbc1dccf4d646b4a297d9ca776b5fc2</t>
         </is>
       </c>
       <c r="J134" t="inlineStr"/>
@@ -29559,7 +29559,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>1a038cb7-de3f-47e8-adff-6dc4867ab197</t>
+          <t>afb8c925-ce16-4258-898b-9c4e9a557d0d</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -29569,7 +29569,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E135" t="inlineStr"/>
@@ -29582,7 +29582,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>https://www.notion.so/134-1a038cb7de3f47e8adff6dc4867ab197</t>
+          <t>https://www.notion.so/134-afb8c925ce164258898b9c4e9a557d0d</t>
         </is>
       </c>
       <c r="J135" t="inlineStr"/>
@@ -29776,7 +29776,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>fb6d55d5-a1f5-4598-8acc-2b0c2bf0f78a</t>
+          <t>1a038cb7-de3f-47e8-adff-6dc4867ab197</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -29786,7 +29786,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E136" t="inlineStr"/>
@@ -29799,7 +29799,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>https://www.notion.so/135-fb6d55d5a1f545988acc2b0c2bf0f78a</t>
+          <t>https://www.notion.so/135-1a038cb7de3f47e8adff6dc4867ab197</t>
         </is>
       </c>
       <c r="J136" t="inlineStr"/>
@@ -29993,7 +29993,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>867d7647-b7a8-43c1-86d4-b05228499271</t>
+          <t>fb6d55d5-a1f5-4598-8acc-2b0c2bf0f78a</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -30003,7 +30003,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2024-07-04T09:46:00.000Z</t>
+          <t>2024-07-06T13:12:00.000Z</t>
         </is>
       </c>
       <c r="E137" t="inlineStr"/>
@@ -30016,7 +30016,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>https://www.notion.so/136-867d7647b7a843c186d4b05228499271</t>
+          <t>https://www.notion.so/136-fb6d55d5a1f545988acc2b0c2bf0f78a</t>
         </is>
       </c>
       <c r="J137" t="inlineStr"/>
@@ -30199,6 +30199,223 @@
       <c r="AY137" t="inlineStr">
         <is>
           <t>[{'type': 'text', 'text': {'content': '136', 'link': None}, 'annotations': {'bold': False, 'italic': False, 'strikethrough': False, 'underline': False, 'code': False, 'color': 'default'}, 'plain_text': '136', 'href': None}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>867d7647-b7a8-43c1-86d4-b05228499271</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2024-06-24T17:11:00.000Z</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2024-07-06T13:12:00.000Z</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr"/>
+      <c r="G138" t="b">
+        <v>0</v>
+      </c>
+      <c r="H138" t="b">
+        <v>0</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/137-867d7647b7a843c186d4b05228499271</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr"/>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P138" t="inlineStr">
+        <is>
+          <t>88e410cc-a410-4367-aad5-55987f9467f7</t>
+        </is>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>IynB</t>
+        </is>
+      </c>
+      <c r="R138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S138" t="n">
+        <v>685000</v>
+      </c>
+      <c r="T138" t="inlineStr">
+        <is>
+          <t>PSic</t>
+        </is>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>formula</t>
+        </is>
+      </c>
+      <c r="V138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="W138" t="n">
+        <v>-685000</v>
+      </c>
+      <c r="X138" t="inlineStr">
+        <is>
+          <t>Uc%3A%5E</t>
+        </is>
+      </c>
+      <c r="Y138" t="inlineStr">
+        <is>
+          <t>formula</t>
+        </is>
+      </c>
+      <c r="Z138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AA138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB138" t="inlineStr">
+        <is>
+          <t>V%3CuY</t>
+        </is>
+      </c>
+      <c r="AC138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AD138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE138" t="inlineStr">
+        <is>
+          <t>%5Be%3DQ</t>
+        </is>
+      </c>
+      <c r="AF138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AG138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH138" t="inlineStr">
+        <is>
+          <t>ccio</t>
+        </is>
+      </c>
+      <c r="AI138" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="AJ138" t="inlineStr">
+        <is>
+          <t>2024-07-06</t>
+        </is>
+      </c>
+      <c r="AK138" t="inlineStr"/>
+      <c r="AL138" t="inlineStr"/>
+      <c r="AM138" t="inlineStr">
+        <is>
+          <t>iRq%5E</t>
+        </is>
+      </c>
+      <c r="AN138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AO138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP138" t="inlineStr">
+        <is>
+          <t>oNis</t>
+        </is>
+      </c>
+      <c r="AQ138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AR138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS138" t="inlineStr">
+        <is>
+          <t>pOIL</t>
+        </is>
+      </c>
+      <c r="AT138" t="inlineStr">
+        <is>
+          <t>formula</t>
+        </is>
+      </c>
+      <c r="AU138" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AV138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW138" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AX138" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AY138" t="inlineStr">
+        <is>
+          <t>[{'type': 'text', 'text': {'content': '137', 'link': None}, 'annotations': {'bold': False, 'italic': False, 'strikethrough': False, 'underline': False, 'code': False, 'color': 'default'}, 'plain_text': '137', 'href': None}]</t>
         </is>
       </c>
     </row>

</xml_diff>